<commit_message>
Benchmarking: adding FFT routines and results
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FIR Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FIR Speed Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="15315" windowHeight="11250" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="15315" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="3" r:id="rId1"/>
@@ -492,7 +492,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.15304642013303429"/>
           <c:y val="0.16714129483814524"/>
-          <c:w val="0.76257425202307094"/>
+          <c:w val="0.56091349791240519"/>
           <c:h val="0.67521216097987746"/>
         </c:manualLayout>
       </c:layout>
@@ -585,10 +585,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Comparison!$B$5:$B$12</c:f>
+              <c:f>Comparison!$B$5:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -612,16 +612,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Comparison!$D$5:$D$12</c:f>
+              <c:f>Comparison!$D$5:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>30.2</c:v>
                 </c:pt>
@@ -645,6 +648,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3761</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -886,6 +892,76 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Python, PC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Comparison!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$H$8:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.6927500000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.3607499999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.7690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.97575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.0565</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.3535</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -894,15 +970,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="138462720"/>
-        <c:axId val="138464640"/>
+        <c:axId val="134063616"/>
+        <c:axId val="134065536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="138462720"/>
+        <c:axId val="134063616"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="512"/>
+          <c:max val="1024"/>
           <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -930,18 +1006,18 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138464640"/>
+        <c:crossAx val="134065536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="138464640"/>
+        <c:axId val="134065536"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1000"/>
-          <c:min val="10"/>
+          <c:max val="10000"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -969,7 +1045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138462720"/>
+        <c:crossAx val="134063616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -982,10 +1058,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.69238015726204705"/>
-          <c:y val="0.48738438806648249"/>
-          <c:w val="0.26242659376517646"/>
-          <c:h val="0.32708209332000465"/>
+          <c:x val="0.74739597052147844"/>
+          <c:y val="0.28192695880538099"/>
+          <c:w val="0.2246035437741101"/>
+          <c:h val="0.46440861222539109"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1324,11 +1400,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="138506240"/>
-        <c:axId val="138507776"/>
+        <c:axId val="134119424"/>
+        <c:axId val="134120960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="138506240"/>
+        <c:axId val="134119424"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1341,12 +1417,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138507776"/>
+        <c:crossAx val="134120960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="138507776"/>
+        <c:axId val="134120960"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1358,13 +1434,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138506240"/>
+        <c:crossAx val="134119424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1616,11 +1693,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="139074176"/>
-        <c:axId val="139075968"/>
+        <c:axId val="142350976"/>
+        <c:axId val="142352768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="139074176"/>
+        <c:axId val="142350976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,7 +1706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139075968"/>
+        <c:crossAx val="142352768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1637,7 +1714,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139075968"/>
+        <c:axId val="142352768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1666,7 +1743,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139074176"/>
+        <c:crossAx val="142350976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1924,11 +2001,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="139102464"/>
-        <c:axId val="139116544"/>
+        <c:axId val="142389248"/>
+        <c:axId val="142390784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="139102464"/>
+        <c:axId val="142389248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1937,7 +2014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139116544"/>
+        <c:crossAx val="142390784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1945,7 +2022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139116544"/>
+        <c:axId val="142390784"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1975,7 +2052,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139102464"/>
+        <c:crossAx val="142389248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2168,11 +2245,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="139131904"/>
-        <c:axId val="139408128"/>
+        <c:axId val="142408704"/>
+        <c:axId val="142680832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="139131904"/>
+        <c:axId val="142408704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,7 +2258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139408128"/>
+        <c:crossAx val="142680832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2189,7 +2266,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139408128"/>
+        <c:axId val="142680832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2226,7 +2303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139131904"/>
+        <c:crossAx val="142408704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -2457,11 +2534,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="139442816"/>
-        <c:axId val="139444608"/>
+        <c:axId val="142715520"/>
+        <c:axId val="142717312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="139442816"/>
+        <c:axId val="142715520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2470,7 +2547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="139444608"/>
+        <c:crossAx val="142717312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2478,7 +2555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139444608"/>
+        <c:axId val="142717312"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2521,7 +2598,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139442816"/>
+        <c:crossAx val="142715520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2690,11 +2767,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="41949440"/>
-        <c:axId val="41947904"/>
+        <c:axId val="134396928"/>
+        <c:axId val="134399104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41949440"/>
+        <c:axId val="134396928"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2724,13 +2801,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="41947904"/>
+        <c:crossAx val="134399104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41947904"/>
+        <c:axId val="134399104"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2761,7 +2838,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41949440"/>
+        <c:crossAx val="134396928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2931,11 +3008,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42461440"/>
-        <c:axId val="42459904"/>
+        <c:axId val="142288384"/>
+        <c:axId val="142290304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42461440"/>
+        <c:axId val="142288384"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2965,13 +3042,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42459904"/>
+        <c:crossAx val="142290304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42459904"/>
+        <c:axId val="142290304"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3002,7 +3079,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42461440"/>
+        <c:crossAx val="142288384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3034,8 +3111,8 @@
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
@@ -3869,8 +3946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M75" sqref="M75"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8012,7 +8089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="L25" sqref="K25:L25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Benchmark: tested on Teensy and Arduino MO
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FIR Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FIR Speed Results.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Arduino M0 Pro" sheetId="1" r:id="rId3"/>
     <sheet name="Maple" sheetId="5" r:id="rId4"/>
     <sheet name="Arduino Due" sheetId="6" r:id="rId5"/>
-    <sheet name="Teensy 3.1" sheetId="7" r:id="rId6"/>
+    <sheet name="Teensy 3.2" sheetId="7" r:id="rId6"/>
     <sheet name="NXP K66" sheetId="9" r:id="rId7"/>
     <sheet name="Python" sheetId="8" r:id="rId8"/>
   </sheets>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="82">
   <si>
     <t>Float</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Maple/Due</t>
   </si>
   <si>
-    <t>96 MHz</t>
-  </si>
-  <si>
     <t>96 MHz, Optimized</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
   </si>
   <si>
     <t>72 MHz, Optimized</t>
-  </si>
-  <si>
-    <t>http://www.pjrc.com/teensy/teensy31.html</t>
   </si>
   <si>
     <t>Teensy 3.1</t>
@@ -262,6 +256,18 @@
   <si>
     <t>int16</t>
   </si>
+  <si>
+    <t>http://www.pjrc.com/store/teensy32.html</t>
+  </si>
+  <si>
+    <t>Teensy 3.2</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>usec / FIR</t>
+  </si>
 </sst>
 </file>
 
@@ -341,112 +347,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -732,22 +633,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>118.3</c:v>
+                  <c:v>114.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>235</c:v>
+                  <c:v>226.47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>473</c:v>
+                  <c:v>446.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>945</c:v>
+                  <c:v>892.74</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1887</c:v>
+                  <c:v>1783.68</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3761</c:v>
+                  <c:v>3567.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,7 +811,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Teensy 3.1</c:v>
+                  <c:v>Teensy 3.2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -949,22 +850,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30.53</c:v>
+                  <c:v>29.24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.01</c:v>
+                  <c:v>58.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124.89</c:v>
+                  <c:v>115.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>250.57</c:v>
+                  <c:v>230.49</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>501.85</c:v>
+                  <c:v>460.29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1004.33</c:v>
+                  <c:v>919.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1119,11 +1020,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116646656"/>
-        <c:axId val="84894848"/>
+        <c:axId val="87657856"/>
+        <c:axId val="87668224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116646656"/>
+        <c:axId val="87657856"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1155,13 +1056,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84894848"/>
+        <c:crossAx val="87668224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84894848"/>
+        <c:axId val="87668224"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1194,7 +1095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116646656"/>
+        <c:crossAx val="87657856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -1337,16 +1238,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>112.4</c:v>
+                  <c:v>114.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>224.49</c:v>
+                  <c:v>226.47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>452.33</c:v>
+                  <c:v>446.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>903.68</c:v>
+                  <c:v>892.74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1431,16 +1332,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13.26</c:v>
+                  <c:v>9.11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.94</c:v>
+                  <c:v>17.46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.96</c:v>
+                  <c:v>34.15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>107.34</c:v>
+                  <c:v>67.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1525,16 +1426,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13.26</c:v>
+                  <c:v>10.77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.94</c:v>
+                  <c:v>20.79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.97</c:v>
+                  <c:v>40.83</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>107.35</c:v>
+                  <c:v>80.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1549,11 +1450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84932096"/>
-        <c:axId val="84933632"/>
+        <c:axId val="87844736"/>
+        <c:axId val="87846272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84932096"/>
+        <c:axId val="87844736"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1566,12 +1467,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84933632"/>
+        <c:crossAx val="87846272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84933632"/>
+        <c:axId val="87846272"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1583,14 +1484,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84932096"/>
+        <c:crossAx val="87844736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1696,7 +1596,7 @@
                   <c:v>622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>224.49</c:v>
+                  <c:v>226.47</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>77.28</c:v>
@@ -1705,7 +1605,7 @@
                   <c:v>71.64</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>62.01</c:v>
+                  <c:v>58.05</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
                   <c:v>2.6</c:v>
@@ -1765,7 +1665,7 @@
                   <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.94</c:v>
+                  <c:v>20.79</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>11.61</c:v>
@@ -1774,7 +1674,7 @@
                   <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>3.82</c:v>
+                  <c:v>4.16</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
                   <c:v>2</c:v>
@@ -1834,7 +1734,7 @@
                   <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.94</c:v>
+                  <c:v>17.46</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>11.61</c:v>
@@ -1843,7 +1743,7 @@
                   <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>3.82</c:v>
+                  <c:v>4.16</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
                   <c:v>2</c:v>
@@ -1861,11 +1761,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="115900800"/>
-        <c:axId val="115902336"/>
+        <c:axId val="87864064"/>
+        <c:axId val="87865600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115900800"/>
+        <c:axId val="87864064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1874,7 +1774,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115902336"/>
+        <c:crossAx val="87865600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1882,7 +1782,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115902336"/>
+        <c:axId val="87865600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,7 +1812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115900800"/>
+        <c:crossAx val="87864064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2026,7 +1926,7 @@
                   <c:v>622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>224.49</c:v>
+                  <c:v>226.47</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>77.28</c:v>
@@ -2035,7 +1935,7 @@
                   <c:v>71.64</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>62.01</c:v>
+                  <c:v>58.05</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
                   <c:v>2.6</c:v>
@@ -2098,7 +1998,7 @@
                   <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.94</c:v>
+                  <c:v>20.79</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>11.61</c:v>
@@ -2107,7 +2007,7 @@
                   <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>3.82</c:v>
+                  <c:v>4.16</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
                   <c:v>2</c:v>
@@ -2170,7 +2070,7 @@
                   <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.94</c:v>
+                  <c:v>17.46</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>11.61</c:v>
@@ -2179,7 +2079,7 @@
                   <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>3.82</c:v>
+                  <c:v>4.16</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
                   <c:v>2</c:v>
@@ -2199,11 +2099,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115929088"/>
-        <c:axId val="115930624"/>
+        <c:axId val="87908352"/>
+        <c:axId val="87909888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115929088"/>
+        <c:axId val="87908352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2212,7 +2112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115930624"/>
+        <c:crossAx val="87909888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2220,7 +2120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115930624"/>
+        <c:axId val="87909888"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2251,7 +2151,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115929088"/>
+        <c:crossAx val="87908352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2371,13 +2271,13 @@
                   <c:v>3549.4260376644552</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5947.4704793272776</c:v>
+                  <c:v>5986.5081443669142</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10561.849922156138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11318.689818636485</c:v>
+                  <c:v>11768.778828946262</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>56011.203361120395</c:v>
@@ -2434,13 +2334,13 @@
                   <c:v>5639.9596744324917</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17218.042770596836</c:v>
+                  <c:v>19795.674375415139</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>25400.025400038103</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46188.021535170061</c:v>
+                  <c:v>44253.636380814365</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>64051.261522034853</c:v>
@@ -2458,11 +2358,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="116739072"/>
-        <c:axId val="116749056"/>
+        <c:axId val="87919232"/>
+        <c:axId val="87933312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116739072"/>
+        <c:axId val="87919232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2471,7 +2371,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116749056"/>
+        <c:crossAx val="87933312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2479,7 +2379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116749056"/>
+        <c:axId val="87933312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2516,7 +2416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116739072"/>
+        <c:crossAx val="87919232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -2638,13 +2538,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8724981467753889</c:v>
+                  <c:v>4.5387994143484631</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.666666666666668</c:v>
+                  <c:v>18.971848225214199</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>39.743589743589745</c:v>
@@ -2704,13 +2604,13 @@
                   <c:v>0.30815109343936381</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8719659069853622</c:v>
+                  <c:v>3.7962282635317171</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.666666666666668</c:v>
+                  <c:v>18.971848225214199</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>39.743589743589745</c:v>
@@ -2770,13 +2670,13 @@
                   <c:v>0.12204724409448819</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34267017443017267</c:v>
+                  <c:v>0.3471833351999104</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0806665272258245</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2410921611017696</c:v>
+                  <c:v>1.3417590027700832</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>30.3921568627451</c:v>
@@ -2796,11 +2696,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135670016"/>
-        <c:axId val="135675904"/>
+        <c:axId val="87968000"/>
+        <c:axId val="87977984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135670016"/>
+        <c:axId val="87968000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2809,7 +2709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="135675904"/>
+        <c:crossAx val="87977984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2817,7 +2717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135675904"/>
+        <c:axId val="87977984"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2860,7 +2760,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135670016"/>
+        <c:crossAx val="87968000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3029,11 +2929,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137415296"/>
-        <c:axId val="137417472"/>
+        <c:axId val="111872640"/>
+        <c:axId val="111878912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137415296"/>
+        <c:axId val="111872640"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3062,13 +2962,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="137417472"/>
+        <c:crossAx val="111878912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137417472"/>
+        <c:axId val="111878912"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3098,7 +2998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137415296"/>
+        <c:crossAx val="111872640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3266,11 +3166,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137704576"/>
-        <c:axId val="137706496"/>
+        <c:axId val="124781696"/>
+        <c:axId val="124783616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137704576"/>
+        <c:axId val="124781696"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3299,13 +3199,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137706496"/>
+        <c:crossAx val="124783616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137706496"/>
+        <c:axId val="124783616"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3335,7 +3235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137704576"/>
+        <c:crossAx val="124781696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3613,14 +3513,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3644,7 +3544,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5991225" y="3324225"/>
+          <a:off x="5991225" y="3638550"/>
           <a:ext cx="3657600" cy="2743200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3791,20 +3691,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>17526</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="http://www.pjrc.com/teensy/teensy31.png"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="http://www.pjrc.com/store/teensy32.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3824,8 +3724,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4257675" y="1038225"/>
-          <a:ext cx="3124200" cy="1762125"/>
+          <a:off x="4648200" y="742950"/>
+          <a:ext cx="3657600" cy="1751076"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4201,8 +4101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4235,13 +4135,13 @@
         <v>Arduino Due</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="H1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="2:17">
@@ -4271,13 +4171,13 @@
       </c>
     </row>
     <row r="3" spans="2:17">
-      <c r="C3" t="str">
-        <f>'Arduino Uno'!I7</f>
-        <v>function</v>
+      <c r="C3">
+        <f>'Arduino Uno'!M10</f>
+        <v>0</v>
       </c>
       <c r="D3" t="str">
-        <f>'Arduino M0 Pro'!C8</f>
-        <v>Function</v>
+        <f>'Arduino M0 Pro'!K7</f>
+        <v>Inline, using types.h</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -4287,7 +4187,7 @@
         <v>Inline, using types.h</v>
       </c>
       <c r="G3" t="str">
-        <f>'Teensy 3.1'!C7</f>
+        <f>'Teensy 3.2'!C19</f>
         <v>96 MHz, Optimized</v>
       </c>
       <c r="H3" t="str">
@@ -4295,7 +4195,7 @@
         <v>Inline, using types.h</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="2:17">
@@ -4324,7 +4224,7 @@
         <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -4336,10 +4236,10 @@
         <v>44</v>
       </c>
       <c r="O4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="2:17">
@@ -4348,11 +4248,12 @@
         <v>4</v>
       </c>
       <c r="C5">
+        <f>'Arduino Uno'!L9</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>'Arduino M0 Pro'!C10</f>
-        <v>30.2</v>
+        <f>'Arduino M0 Pro'!K10</f>
+        <v>0</v>
       </c>
       <c r="E5">
         <f>Maple!D9</f>
@@ -4363,17 +4264,16 @@
         <v>8.61</v>
       </c>
       <c r="G5">
-        <f>'Teensy 3.1'!D9</f>
-        <v>6.81</v>
+        <v>0</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10">
         <f>Python!D9</f>
         <v>5.698666666666667</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="10" t="e">
         <f t="shared" ref="L5" si="0">C5/D5</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ref="M5" si="1">C5/E5</f>
@@ -4383,9 +4283,9 @@
         <f>$C5/F5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="10" t="e">
         <f>$C5/G5</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10">
@@ -4399,11 +4299,12 @@
         <v>8</v>
       </c>
       <c r="C6">
+        <f>'Arduino Uno'!L10</f>
         <v>0</v>
       </c>
       <c r="D6">
-        <f>'Arduino M0 Pro'!C11</f>
-        <v>59.57</v>
+        <f>'Arduino M0 Pro'!K11</f>
+        <v>59.51</v>
       </c>
       <c r="E6">
         <f>Maple!D10</f>
@@ -4414,8 +4315,8 @@
         <v>17.670000000000002</v>
       </c>
       <c r="G6">
-        <f>'Teensy 3.1'!D10</f>
-        <v>14.74</v>
+        <f>'Teensy 3.2'!C6</f>
+        <v>14.87</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10">
@@ -4454,8 +4355,8 @@
         <v>311</v>
       </c>
       <c r="D7">
-        <f>'Arduino M0 Pro'!C12</f>
-        <v>118.3</v>
+        <f>'Arduino M0 Pro'!K12</f>
+        <v>114.83</v>
       </c>
       <c r="E7">
         <f>Maple!D11</f>
@@ -4466,8 +4367,8 @@
         <v>35.69</v>
       </c>
       <c r="G7">
-        <f>'Teensy 3.1'!D11</f>
-        <v>30.53</v>
+        <f>'Teensy 3.2'!C7</f>
+        <v>29.24</v>
       </c>
       <c r="H7" s="10">
         <f>'NXP K66'!D11</f>
@@ -4478,12 +4379,12 @@
         <v>5.5045000000000002</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K6:K10" si="6">C7/C7</f>
+        <f t="shared" ref="K7:K10" si="6">C7/C7</f>
         <v>1</v>
       </c>
       <c r="L7" s="10">
         <f t="shared" si="2"/>
-        <v>2.6289095519864749</v>
+        <v>2.7083514760950971</v>
       </c>
       <c r="M7" s="10">
         <f t="shared" si="3"/>
@@ -4495,7 +4396,7 @@
       </c>
       <c r="O7" s="10">
         <f>$C7/G7</f>
-        <v>10.186701604978708</v>
+        <v>10.636114911080712</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10">
@@ -4513,8 +4414,8 @@
         <v>622</v>
       </c>
       <c r="D8">
-        <f>'Arduino M0 Pro'!C13</f>
-        <v>235</v>
+        <f>'Arduino M0 Pro'!K13</f>
+        <v>226.47</v>
       </c>
       <c r="E8">
         <f>Maple!D12</f>
@@ -4525,8 +4426,8 @@
         <v>71.64</v>
       </c>
       <c r="G8">
-        <f>'Teensy 3.1'!D12</f>
-        <v>62.01</v>
+        <f>'Teensy 3.2'!C8</f>
+        <v>58.05</v>
       </c>
       <c r="H8" s="10">
         <f>'NXP K66'!D12</f>
@@ -4542,7 +4443,7 @@
       </c>
       <c r="L8" s="10">
         <f t="shared" si="2"/>
-        <v>2.6468085106382979</v>
+        <v>2.7465006402614032</v>
       </c>
       <c r="M8" s="10">
         <f t="shared" si="3"/>
@@ -4554,7 +4455,7 @@
       </c>
       <c r="O8" s="10">
         <f>$C8/G8</f>
-        <v>10.030640219319466</v>
+        <v>10.714900947459087</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="10">
@@ -4572,8 +4473,8 @@
         <v>1270</v>
       </c>
       <c r="D9">
-        <f>'Arduino M0 Pro'!C14</f>
-        <v>473</v>
+        <f>'Arduino M0 Pro'!K14</f>
+        <v>446.45</v>
       </c>
       <c r="E9">
         <f>Maple!D13</f>
@@ -4584,8 +4485,8 @@
         <v>143.43</v>
       </c>
       <c r="G9">
-        <f>'Teensy 3.1'!D13</f>
-        <v>124.89</v>
+        <f>'Teensy 3.2'!C9</f>
+        <v>115.52</v>
       </c>
       <c r="H9" s="10">
         <f>'NXP K66'!D13</f>
@@ -4601,7 +4502,7 @@
       </c>
       <c r="L9" s="10">
         <f t="shared" si="2"/>
-        <v>2.6849894291754759</v>
+        <v>2.8446634561541049</v>
       </c>
       <c r="M9" s="10">
         <f t="shared" si="3"/>
@@ -4613,7 +4514,7 @@
       </c>
       <c r="O9" s="10">
         <f>$C9/G9</f>
-        <v>10.168948674833853</v>
+        <v>10.993767313019392</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="10">
@@ -4631,8 +4532,8 @@
         <v>2522</v>
       </c>
       <c r="D10">
-        <f>'Arduino M0 Pro'!C15</f>
-        <v>945</v>
+        <f>'Arduino M0 Pro'!K15</f>
+        <v>892.74</v>
       </c>
       <c r="E10">
         <f>Maple!D14</f>
@@ -4643,8 +4544,8 @@
         <v>286.93</v>
       </c>
       <c r="G10">
-        <f>'Teensy 3.1'!D14</f>
-        <v>250.57</v>
+        <f>'Teensy 3.2'!C10</f>
+        <v>230.49</v>
       </c>
       <c r="H10" s="10">
         <f>'NXP K66'!D14</f>
@@ -4660,7 +4561,7 @@
       </c>
       <c r="L10" s="10">
         <f t="shared" si="2"/>
-        <v>2.6687830687830689</v>
+        <v>2.8250106413961511</v>
       </c>
       <c r="M10" s="10">
         <f t="shared" si="3"/>
@@ -4672,7 +4573,7 @@
       </c>
       <c r="O10" s="10">
         <f>$C10/G10</f>
-        <v>10.065051682164665</v>
+        <v>10.941906373378455</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="10">
@@ -4685,9 +4586,13 @@
         <f>'Arduino M0 Pro'!B16</f>
         <v>256</v>
       </c>
+      <c r="C11">
+        <f>'Arduino Uno'!L15</f>
+        <v>0</v>
+      </c>
       <c r="D11">
-        <f>'Arduino M0 Pro'!C16</f>
-        <v>1887</v>
+        <f>'Arduino M0 Pro'!K16</f>
+        <v>1783.68</v>
       </c>
       <c r="E11">
         <f>Maple!D15</f>
@@ -4698,8 +4603,8 @@
         <v>573.83000000000004</v>
       </c>
       <c r="G11">
-        <f>'Teensy 3.1'!D15</f>
-        <v>501.85</v>
+        <f>'Teensy 3.2'!C11</f>
+        <v>460.29</v>
       </c>
       <c r="H11" s="10">
         <f>'NXP K66'!D15</f>
@@ -4721,9 +4626,13 @@
         <f>'Arduino M0 Pro'!B17</f>
         <v>512</v>
       </c>
+      <c r="C12">
+        <f>'Arduino Uno'!L16</f>
+        <v>0</v>
+      </c>
       <c r="D12">
-        <f>'Arduino M0 Pro'!C17</f>
-        <v>3761</v>
+        <f>'Arduino M0 Pro'!K17</f>
+        <v>3567.42</v>
       </c>
       <c r="E12">
         <f>Maple!D16</f>
@@ -4734,8 +4643,8 @@
         <v>1147.53</v>
       </c>
       <c r="G12">
-        <f>'Teensy 3.1'!D16</f>
-        <v>1004.33</v>
+        <f>'Teensy 3.2'!C12</f>
+        <v>919.99</v>
       </c>
       <c r="H12" s="10">
         <f>'NXP K66'!D16</f>
@@ -4751,9 +4660,13 @@
         <f>'Arduino M0 Pro'!B18</f>
         <v>1024</v>
       </c>
+      <c r="C13">
+        <f>'Arduino Uno'!L17</f>
+        <v>0</v>
+      </c>
       <c r="D13">
-        <f>'Arduino M0 Pro'!C18</f>
-        <v>7519</v>
+        <f>'Arduino M0 Pro'!K18</f>
+        <v>7131.84</v>
       </c>
       <c r="H13" s="10">
         <f>'NXP K66'!D17</f>
@@ -4882,7 +4795,7 @@
         <v>Arduino Due</v>
       </c>
       <c r="G23" t="str">
-        <f>'Teensy 3.1'!C6</f>
+        <f>'Teensy 3.2'!C18</f>
         <v>Teensy 3.1</v>
       </c>
       <c r="H23" t="str">
@@ -4972,7 +4885,7 @@
         <v>Inline, using types.h</v>
       </c>
       <c r="G24" t="str">
-        <f>'Teensy 3.1'!C7</f>
+        <f>'Teensy 3.2'!C19</f>
         <v>96 MHz, Optimized</v>
       </c>
       <c r="H24" t="str">
@@ -5010,7 +4923,7 @@
         <v>21</v>
       </c>
       <c r="K25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L25" t="s">
         <v>28</v>
@@ -5022,13 +4935,13 @@
         <v>44</v>
       </c>
       <c r="O25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S25" t="s">
         <v>30</v>
@@ -5037,10 +4950,10 @@
         <v>45</v>
       </c>
       <c r="U25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="V25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="X25" t="s">
         <v>25</v>
@@ -5076,7 +4989,7 @@
       </c>
       <c r="D26" s="4">
         <f>'Arduino M0 Pro'!K12</f>
-        <v>112.4</v>
+        <v>114.83</v>
       </c>
       <c r="E26">
         <f>Maple!D11</f>
@@ -5087,8 +5000,8 @@
         <v>35.69</v>
       </c>
       <c r="G26">
-        <f>'Teensy 3.1'!D11</f>
-        <v>30.53</v>
+        <f>'Teensy 3.2'!C7</f>
+        <v>29.24</v>
       </c>
       <c r="H26" s="10">
         <f>'NXP K66'!D11</f>
@@ -5104,7 +5017,7 @@
       </c>
       <c r="L26" s="6">
         <f t="shared" ref="L26:L37" si="9">C26/D26</f>
-        <v>2.7669039145907472</v>
+        <v>2.7083514760950971</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" ref="M26:M37" si="10">C26/E26</f>
@@ -5116,7 +5029,7 @@
       </c>
       <c r="O26" s="6">
         <f>$C26/G26</f>
-        <v>10.186701604978708</v>
+        <v>10.636114911080712</v>
       </c>
       <c r="P26" s="6">
         <f>C26/H26</f>
@@ -5129,7 +5042,7 @@
       <c r="R26" s="6"/>
       <c r="S26" s="6">
         <f t="shared" ref="S26:S37" si="11">D26/E26</f>
-        <v>2.9240374609781479</v>
+        <v>2.9872528616024976</v>
       </c>
       <c r="T26" s="6">
         <f t="shared" ref="T26:T37" si="12">E26/F26</f>
@@ -5137,11 +5050,11 @@
       </c>
       <c r="U26" s="6">
         <f t="shared" ref="U26:U37" si="13">E26/G26</f>
-        <v>1.2590894202423843</v>
+        <v>1.3146374829001368</v>
       </c>
       <c r="V26" s="6">
         <f>G26/H26</f>
-        <v>23.484615384615385</v>
+        <v>22.492307692307691</v>
       </c>
       <c r="W26" s="6"/>
       <c r="X26" s="6">
@@ -5150,7 +5063,7 @@
       </c>
       <c r="Y26" s="6">
         <f t="shared" si="14"/>
-        <v>8.4766214177978885</v>
+        <v>12.604829857299672</v>
       </c>
       <c r="Z26" s="6">
         <f t="shared" si="14"/>
@@ -5162,7 +5075,7 @@
       </c>
       <c r="AB26" s="6">
         <f t="shared" si="14"/>
-        <v>15.341708542713569</v>
+        <v>13.537037037037035</v>
       </c>
       <c r="AC26" s="6">
         <f t="shared" si="14"/>
@@ -5180,7 +5093,7 @@
       </c>
       <c r="D27" s="4">
         <f>'Arduino M0 Pro'!K13</f>
-        <v>224.49</v>
+        <v>226.47</v>
       </c>
       <c r="E27">
         <f>Maple!D12</f>
@@ -5191,8 +5104,8 @@
         <v>71.64</v>
       </c>
       <c r="G27">
-        <f>'Teensy 3.1'!D12</f>
-        <v>62.01</v>
+        <f>'Teensy 3.2'!C8</f>
+        <v>58.05</v>
       </c>
       <c r="H27" s="10">
         <f>'NXP K66'!D12</f>
@@ -5208,7 +5121,7 @@
       </c>
       <c r="L27" s="6">
         <f t="shared" si="9"/>
-        <v>2.7707247538865873</v>
+        <v>2.7465006402614032</v>
       </c>
       <c r="M27" s="6">
         <f t="shared" si="10"/>
@@ -5220,7 +5133,7 @@
       </c>
       <c r="O27" s="6">
         <f t="shared" ref="O27:O37" si="19">$C27/G27</f>
-        <v>10.030640219319466</v>
+        <v>10.714900947459087</v>
       </c>
       <c r="P27" s="6">
         <f t="shared" ref="P27:P37" si="20">C27/H27</f>
@@ -5233,7 +5146,7 @@
       <c r="R27" s="6"/>
       <c r="S27" s="6">
         <f t="shared" si="11"/>
-        <v>2.9048913043478262</v>
+        <v>2.9305124223602483</v>
       </c>
       <c r="T27" s="6">
         <f t="shared" si="12"/>
@@ -5241,11 +5154,11 @@
       </c>
       <c r="U27" s="6">
         <f t="shared" si="13"/>
-        <v>1.2462506047411708</v>
+        <v>1.3312661498708012</v>
       </c>
       <c r="V27" s="6">
         <f t="shared" ref="V27:V37" si="22">G27/H27</f>
-        <v>23.849999999999998</v>
+        <v>22.326923076923077</v>
       </c>
       <c r="W27" s="6"/>
       <c r="X27" s="6">
@@ -5254,7 +5167,7 @@
       </c>
       <c r="Y27" s="6">
         <f t="shared" si="23"/>
-        <v>8.6542020046260593</v>
+        <v>12.970790378006873</v>
       </c>
       <c r="Z27" s="6">
         <f t="shared" si="23"/>
@@ -5266,7 +5179,7 @@
       </c>
       <c r="AB27" s="6">
         <f t="shared" ref="AB27:AC29" si="24">G27/G35</f>
-        <v>16.232984293193716</v>
+        <v>13.954326923076922</v>
       </c>
       <c r="AC27" s="6">
         <f t="shared" si="24"/>
@@ -5284,7 +5197,7 @@
       </c>
       <c r="D28" s="4">
         <f>'Arduino M0 Pro'!K14</f>
-        <v>452.33</v>
+        <v>446.45</v>
       </c>
       <c r="E28">
         <f>Maple!D13</f>
@@ -5295,8 +5208,8 @@
         <v>143.43</v>
       </c>
       <c r="G28">
-        <f>'Teensy 3.1'!D13</f>
-        <v>124.89</v>
+        <f>'Teensy 3.2'!C9</f>
+        <v>115.52</v>
       </c>
       <c r="H28" s="10">
         <f>'NXP K66'!D13</f>
@@ -5312,7 +5225,7 @@
       </c>
       <c r="L28" s="6">
         <f t="shared" si="9"/>
-        <v>2.8076846550085115</v>
+        <v>2.8446634561541049</v>
       </c>
       <c r="M28" s="6">
         <f t="shared" si="10"/>
@@ -5324,7 +5237,7 @@
       </c>
       <c r="O28" s="6">
         <f t="shared" si="19"/>
-        <v>10.168948674833853</v>
+        <v>10.993767313019392</v>
       </c>
       <c r="P28" s="6">
         <f t="shared" si="20"/>
@@ -5337,7 +5250,7 @@
       <c r="R28" s="6"/>
       <c r="S28" s="6">
         <f t="shared" si="11"/>
-        <v>2.9197650400206561</v>
+        <v>2.8818099664342887</v>
       </c>
       <c r="T28" s="6">
         <f t="shared" si="12"/>
@@ -5345,11 +5258,11 @@
       </c>
       <c r="U28" s="6">
         <f t="shared" si="13"/>
-        <v>1.2404515974057169</v>
+        <v>1.3410664819944598</v>
       </c>
       <c r="V28" s="6">
         <f t="shared" si="22"/>
-        <v>24.488235294117651</v>
+        <v>22.650980392156864</v>
       </c>
       <c r="W28" s="6"/>
       <c r="X28" s="6">
@@ -5358,7 +5271,7 @@
       </c>
       <c r="Y28" s="6">
         <f t="shared" si="23"/>
-        <v>8.3826908821349146</v>
+        <v>13.07320644216691</v>
       </c>
       <c r="Z28" s="6">
         <f t="shared" si="23"/>
@@ -5370,7 +5283,7 @@
       </c>
       <c r="AB28" s="6">
         <f t="shared" si="24"/>
-        <v>16.652000000000001</v>
+        <v>14.13953488372093</v>
       </c>
       <c r="AC28" s="6">
         <f t="shared" si="24"/>
@@ -5388,7 +5301,7 @@
       </c>
       <c r="D29" s="4">
         <f>'Arduino M0 Pro'!K15</f>
-        <v>903.68</v>
+        <v>892.74</v>
       </c>
       <c r="E29">
         <f>Maple!D14</f>
@@ -5399,8 +5312,8 @@
         <v>286.93</v>
       </c>
       <c r="G29">
-        <f>'Teensy 3.1'!D14</f>
-        <v>250.57</v>
+        <f>'Teensy 3.2'!C10</f>
+        <v>230.49</v>
       </c>
       <c r="H29" s="10">
         <f>'NXP K66'!D14</f>
@@ -5416,7 +5329,7 @@
       </c>
       <c r="L29" s="6">
         <f t="shared" si="9"/>
-        <v>2.7908109065155808</v>
+        <v>2.8250106413961511</v>
       </c>
       <c r="M29" s="6">
         <f t="shared" si="10"/>
@@ -5428,7 +5341,7 @@
       </c>
       <c r="O29" s="6">
         <f t="shared" si="19"/>
-        <v>10.065051682164665</v>
+        <v>10.941906373378455</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="20"/>
@@ -5441,7 +5354,7 @@
       <c r="R29" s="6"/>
       <c r="S29" s="6">
         <f t="shared" si="11"/>
-        <v>2.9136869256811222</v>
+        <v>2.8784136708044499</v>
       </c>
       <c r="T29" s="6">
         <f t="shared" si="12"/>
@@ -5449,11 +5362,11 @@
       </c>
       <c r="U29" s="6">
         <f t="shared" si="13"/>
-        <v>1.237777866464461</v>
+        <v>1.3456115232764978</v>
       </c>
       <c r="V29" s="6">
         <f t="shared" si="22"/>
-        <v>25.056999999999999</v>
+        <v>23.048999999999999</v>
       </c>
       <c r="W29" s="6"/>
       <c r="X29" s="6">
@@ -5462,7 +5375,7 @@
       </c>
       <c r="Y29" s="6">
         <f t="shared" si="23"/>
-        <v>8.4188559716787772</v>
+        <v>13.215988156920799</v>
       </c>
       <c r="Z29" s="6">
         <f t="shared" si="23"/>
@@ -5474,7 +5387,7 @@
       </c>
       <c r="AB29" s="6">
         <f t="shared" si="24"/>
-        <v>16.873400673400674</v>
+        <v>14.22777777777778</v>
       </c>
       <c r="AC29" s="6">
         <f t="shared" si="24"/>
@@ -5483,7 +5396,7 @@
     </row>
     <row r="30" spans="1:29">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30">
         <f>B26</f>
@@ -5495,7 +5408,7 @@
       </c>
       <c r="D30" s="4">
         <f>'Arduino M0 Pro'!M12</f>
-        <v>13.26</v>
+        <v>10.77</v>
       </c>
       <c r="E30">
         <f>Maple!E11</f>
@@ -5506,8 +5419,8 @@
         <v>6.49</v>
       </c>
       <c r="G30">
-        <f>'Teensy 3.1'!E11</f>
-        <v>1.99</v>
+        <f>'Teensy 3.2'!D7</f>
+        <v>2.16</v>
       </c>
       <c r="H30" s="10">
         <f>H34</f>
@@ -5523,7 +5436,7 @@
       </c>
       <c r="L30" s="6">
         <f t="shared" si="9"/>
-        <v>9.7285067873303177</v>
+        <v>11.977715877437326</v>
       </c>
       <c r="M30" s="6">
         <f t="shared" si="10"/>
@@ -5535,7 +5448,7 @@
       </c>
       <c r="O30" s="6">
         <f t="shared" si="19"/>
-        <v>64.824120603015075</v>
+        <v>59.722222222222221</v>
       </c>
       <c r="P30" s="6">
         <f t="shared" si="20"/>
@@ -5548,7 +5461,7 @@
       <c r="R30" s="6"/>
       <c r="S30" s="6">
         <f t="shared" si="11"/>
-        <v>2.1953642384105958</v>
+        <v>1.7831125827814569</v>
       </c>
       <c r="T30" s="6">
         <f t="shared" si="12"/>
@@ -5556,11 +5469,11 @@
       </c>
       <c r="U30" s="6">
         <f t="shared" si="13"/>
-        <v>3.0351758793969847</v>
+        <v>2.7962962962962963</v>
       </c>
       <c r="V30" s="6">
         <f t="shared" si="22"/>
-        <v>1.8090909090909089</v>
+        <v>1.9636363636363636</v>
       </c>
       <c r="W30" s="6"/>
       <c r="X30" s="6">
@@ -5569,7 +5482,7 @@
       </c>
       <c r="Y30" s="6">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>1.1822173435784853</v>
       </c>
       <c r="Z30" s="6">
         <f t="shared" si="25"/>
@@ -5599,7 +5512,7 @@
       </c>
       <c r="D31" s="4">
         <f>'Arduino M0 Pro'!M13</f>
-        <v>25.94</v>
+        <v>20.79</v>
       </c>
       <c r="E31">
         <f>Maple!E12</f>
@@ -5610,8 +5523,8 @@
         <v>12.6</v>
       </c>
       <c r="G31">
-        <f>'Teensy 3.1'!E12</f>
-        <v>3.82</v>
+        <f>'Teensy 3.2'!D8</f>
+        <v>4.16</v>
       </c>
       <c r="H31" s="10">
         <f t="shared" ref="H31:H33" si="27">H35</f>
@@ -5627,7 +5540,7 @@
       </c>
       <c r="L31" s="6">
         <f t="shared" si="9"/>
-        <v>9.7918272937548192</v>
+        <v>12.217412217412218</v>
       </c>
       <c r="M31" s="6">
         <f t="shared" si="10"/>
@@ -5639,7 +5552,7 @@
       </c>
       <c r="O31" s="6">
         <f t="shared" si="19"/>
-        <v>66.492146596858646</v>
+        <v>61.057692307692307</v>
       </c>
       <c r="P31" s="6">
         <f t="shared" si="20"/>
@@ -5652,7 +5565,7 @@
       <c r="R31" s="6"/>
       <c r="S31" s="6">
         <f t="shared" si="11"/>
-        <v>2.2342807924203276</v>
+        <v>1.7906976744186047</v>
       </c>
       <c r="T31" s="6">
         <f t="shared" si="12"/>
@@ -5660,11 +5573,11 @@
       </c>
       <c r="U31" s="6">
         <f t="shared" si="13"/>
-        <v>3.0392670157068062</v>
+        <v>2.7908653846153846</v>
       </c>
       <c r="V31" s="6">
         <f t="shared" si="22"/>
-        <v>1.91</v>
+        <v>2.08</v>
       </c>
       <c r="W31" s="6"/>
       <c r="X31" s="6">
@@ -5673,7 +5586,7 @@
       </c>
       <c r="Y31" s="6">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>1.1907216494845361</v>
       </c>
       <c r="Z31" s="6">
         <f t="shared" si="29"/>
@@ -5703,7 +5616,7 @@
       </c>
       <c r="D32" s="4">
         <f>'Arduino M0 Pro'!M14</f>
-        <v>53.97</v>
+        <v>40.83</v>
       </c>
       <c r="E32">
         <f>Maple!E13</f>
@@ -5714,8 +5627,8 @@
         <v>24.8</v>
       </c>
       <c r="G32">
-        <f>'Teensy 3.1'!E13</f>
-        <v>7.5</v>
+        <f>'Teensy 3.2'!D9</f>
+        <v>8.17</v>
       </c>
       <c r="H32" s="10">
         <f t="shared" si="27"/>
@@ -5731,7 +5644,7 @@
       </c>
       <c r="L32" s="6">
         <f t="shared" si="9"/>
-        <v>9.3199925884750794</v>
+        <v>12.319373010041637</v>
       </c>
       <c r="M32" s="6">
         <f t="shared" si="10"/>
@@ -5743,7 +5656,7 @@
       </c>
       <c r="O32" s="6">
         <f t="shared" si="19"/>
-        <v>67.066666666666663</v>
+        <v>61.566707466340269</v>
       </c>
       <c r="P32" s="6">
         <f t="shared" si="20"/>
@@ -5756,7 +5669,7 @@
       <c r="R32" s="6"/>
       <c r="S32" s="6">
         <f t="shared" si="11"/>
-        <v>2.3712653778558872</v>
+        <v>1.7939367311072054</v>
       </c>
       <c r="T32" s="6">
         <f t="shared" si="12"/>
@@ -5764,11 +5677,11 @@
       </c>
       <c r="U32" s="6">
         <f t="shared" si="13"/>
-        <v>3.0346666666666668</v>
+        <v>2.7858017135862916</v>
       </c>
       <c r="V32" s="6">
         <f t="shared" si="22"/>
-        <v>1.9230769230769231</v>
+        <v>2.094871794871795</v>
       </c>
       <c r="W32" s="6"/>
       <c r="X32" s="6">
@@ -5777,7 +5690,7 @@
       </c>
       <c r="Y32" s="6">
         <f t="shared" si="29"/>
-        <v>1.0001853224610822</v>
+        <v>1.1956076134699853</v>
       </c>
       <c r="Z32" s="6">
         <f t="shared" si="29"/>
@@ -5807,7 +5720,7 @@
       </c>
       <c r="D33" s="4">
         <f>'Arduino M0 Pro'!M15</f>
-        <v>107.35</v>
+        <v>80.91</v>
       </c>
       <c r="E33">
         <f>Maple!E14</f>
@@ -5818,8 +5731,8 @@
         <v>49.21</v>
       </c>
       <c r="G33">
-        <f>'Teensy 3.1'!E14</f>
-        <v>14.85</v>
+        <f>'Teensy 3.2'!D10</f>
+        <v>16.2</v>
       </c>
       <c r="H33" s="10">
         <f t="shared" si="27"/>
@@ -5835,7 +5748,7 @@
       </c>
       <c r="L33" s="6">
         <f t="shared" si="9"/>
-        <v>9.3339543549138337</v>
+        <v>12.384130515387469</v>
       </c>
       <c r="M33" s="6">
         <f t="shared" si="10"/>
@@ -5847,7 +5760,7 @@
       </c>
       <c r="O33" s="6">
         <f t="shared" si="19"/>
-        <v>67.474747474747474</v>
+        <v>61.851851851851855</v>
       </c>
       <c r="P33" s="6">
         <f t="shared" si="20"/>
@@ -5860,7 +5773,7 @@
       <c r="R33" s="6"/>
       <c r="S33" s="6">
         <f t="shared" si="11"/>
-        <v>2.3823790501553481</v>
+        <v>1.79560585885486</v>
       </c>
       <c r="T33" s="6">
         <f t="shared" si="12"/>
@@ -5868,11 +5781,11 @@
       </c>
       <c r="U33" s="6">
         <f t="shared" si="13"/>
-        <v>3.0343434343434348</v>
+        <v>2.7814814814814817</v>
       </c>
       <c r="V33" s="6">
         <f t="shared" si="22"/>
-        <v>1.9038461538461537</v>
+        <v>2.0769230769230771</v>
       </c>
       <c r="W33" s="6"/>
       <c r="X33" s="6">
@@ -5881,7 +5794,7 @@
       </c>
       <c r="Y33" s="6">
         <f t="shared" si="29"/>
-        <v>1.000093161915409</v>
+        <v>1.197779422649889</v>
       </c>
       <c r="Z33" s="6">
         <f t="shared" si="29"/>
@@ -5902,7 +5815,7 @@
     </row>
     <row r="34" spans="1:29">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B34">
         <f t="shared" si="26"/>
@@ -5914,7 +5827,7 @@
       </c>
       <c r="D34" s="4">
         <f>'Arduino M0 Pro'!L12</f>
-        <v>13.26</v>
+        <v>9.11</v>
       </c>
       <c r="E34">
         <f>Maple!F11</f>
@@ -5925,8 +5838,8 @@
         <v>6.49</v>
       </c>
       <c r="G34">
-        <f>'Teensy 3.1'!F11</f>
-        <v>1.99</v>
+        <f>G30</f>
+        <v>2.16</v>
       </c>
       <c r="H34" s="10">
         <f>'NXP K66'!F11</f>
@@ -5942,7 +5855,7 @@
       </c>
       <c r="L34" s="6">
         <f t="shared" si="9"/>
-        <v>3.0920060331825039</v>
+        <v>4.5005488474204176</v>
       </c>
       <c r="M34" s="6">
         <f t="shared" si="10"/>
@@ -5954,7 +5867,7 @@
       </c>
       <c r="O34" s="6">
         <f t="shared" si="19"/>
-        <v>20.603015075376884</v>
+        <v>18.981481481481481</v>
       </c>
       <c r="P34" s="6">
         <f t="shared" si="20"/>
@@ -5967,7 +5880,7 @@
       <c r="R34" s="6"/>
       <c r="S34" s="6">
         <f t="shared" si="11"/>
-        <v>2.1953642384105958</v>
+        <v>1.5082781456953642</v>
       </c>
       <c r="T34" s="6">
         <f t="shared" si="12"/>
@@ -5975,11 +5888,11 @@
       </c>
       <c r="U34" s="6">
         <f t="shared" si="13"/>
-        <v>3.0351758793969847</v>
+        <v>2.7962962962962963</v>
       </c>
       <c r="V34" s="6">
         <f t="shared" si="22"/>
-        <v>1.8090909090909089</v>
+        <v>1.9636363636363636</v>
       </c>
       <c r="W34" s="6"/>
       <c r="X34" s="6"/>
@@ -5998,7 +5911,7 @@
       </c>
       <c r="D35" s="4">
         <f>'Arduino M0 Pro'!L13</f>
-        <v>25.94</v>
+        <v>17.46</v>
       </c>
       <c r="E35">
         <f>Maple!F12</f>
@@ -6009,15 +5922,15 @@
         <v>12.6</v>
       </c>
       <c r="G35">
-        <f>'Teensy 3.1'!F12</f>
-        <v>3.82</v>
+        <f t="shared" ref="G35:G37" si="31">G31</f>
+        <v>4.16</v>
       </c>
       <c r="H35" s="10">
         <f>'NXP K66'!F12</f>
         <v>2</v>
       </c>
       <c r="I35" s="10">
-        <f t="shared" ref="I35:I37" si="31">I27</f>
+        <f t="shared" ref="I35:I37" si="32">I27</f>
         <v>5.6927500000000002</v>
       </c>
       <c r="K35">
@@ -6026,7 +5939,7 @@
       </c>
       <c r="L35" s="6">
         <f t="shared" si="9"/>
-        <v>3.0454895913646878</v>
+        <v>4.5246277205040091</v>
       </c>
       <c r="M35" s="6">
         <f t="shared" si="10"/>
@@ -6038,7 +5951,7 @@
       </c>
       <c r="O35" s="6">
         <f t="shared" si="19"/>
-        <v>20.680628272251308</v>
+        <v>18.990384615384613</v>
       </c>
       <c r="P35" s="6">
         <f t="shared" si="20"/>
@@ -6051,7 +5964,7 @@
       <c r="R35" s="6"/>
       <c r="S35" s="6">
         <f t="shared" si="11"/>
-        <v>2.2342807924203276</v>
+        <v>1.5038759689922483</v>
       </c>
       <c r="T35" s="6">
         <f t="shared" si="12"/>
@@ -6059,11 +5972,11 @@
       </c>
       <c r="U35" s="6">
         <f t="shared" si="13"/>
-        <v>3.0392670157068062</v>
+        <v>2.7908653846153846</v>
       </c>
       <c r="V35" s="6">
         <f t="shared" si="22"/>
-        <v>1.91</v>
+        <v>2.08</v>
       </c>
       <c r="W35" s="6"/>
       <c r="X35" s="6"/>
@@ -6082,7 +5995,7 @@
       </c>
       <c r="D36" s="4">
         <f>'Arduino M0 Pro'!L14</f>
-        <v>53.96</v>
+        <v>34.15</v>
       </c>
       <c r="E36">
         <f>Maple!F13</f>
@@ -6093,15 +6006,15 @@
         <v>24.8</v>
       </c>
       <c r="G36">
-        <f>'Teensy 3.1'!F13</f>
-        <v>7.5</v>
+        <f t="shared" si="31"/>
+        <v>8.17</v>
       </c>
       <c r="H36" s="10">
         <f>'NXP K66'!F13</f>
         <v>3.9</v>
       </c>
       <c r="I36" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>8.3607499999999995</v>
       </c>
       <c r="K36">
@@ -6110,7 +6023,7 @@
       </c>
       <c r="L36" s="6">
         <f t="shared" si="9"/>
-        <v>2.8724981467753889</v>
+        <v>4.5387994143484631</v>
       </c>
       <c r="M36" s="6">
         <f t="shared" si="10"/>
@@ -6122,7 +6035,7 @@
       </c>
       <c r="O36" s="6">
         <f t="shared" si="19"/>
-        <v>20.666666666666668</v>
+        <v>18.971848225214199</v>
       </c>
       <c r="P36" s="6">
         <f t="shared" si="20"/>
@@ -6135,7 +6048,7 @@
       <c r="R36" s="6"/>
       <c r="S36" s="6">
         <f t="shared" si="11"/>
-        <v>2.3708260105448153</v>
+        <v>1.5004393673110719</v>
       </c>
       <c r="T36" s="6">
         <f t="shared" si="12"/>
@@ -6143,11 +6056,11 @@
       </c>
       <c r="U36" s="6">
         <f t="shared" si="13"/>
-        <v>3.0346666666666668</v>
+        <v>2.7858017135862916</v>
       </c>
       <c r="V36" s="6">
         <f t="shared" si="22"/>
-        <v>1.9230769230769231</v>
+        <v>2.094871794871795</v>
       </c>
       <c r="W36" s="6"/>
       <c r="X36" s="6"/>
@@ -6166,7 +6079,7 @@
       </c>
       <c r="D37" s="4">
         <f>'Arduino M0 Pro'!L15</f>
-        <v>107.34</v>
+        <v>67.55</v>
       </c>
       <c r="E37">
         <f>Maple!F14</f>
@@ -6177,15 +6090,15 @@
         <v>49.21</v>
       </c>
       <c r="G37">
-        <f>'Teensy 3.1'!F14</f>
-        <v>14.85</v>
+        <f t="shared" si="31"/>
+        <v>16.2</v>
       </c>
       <c r="H37" s="10">
         <f>'NXP K66'!F14</f>
         <v>7.8</v>
       </c>
       <c r="I37" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>8.7690000000000001</v>
       </c>
       <c r="K37">
@@ -6194,7 +6107,7 @@
       </c>
       <c r="L37" s="6">
         <f t="shared" si="9"/>
-        <v>2.8693869945966086</v>
+        <v>4.5595854922279795</v>
       </c>
       <c r="M37" s="6">
         <f t="shared" si="10"/>
@@ -6206,7 +6119,7 @@
       </c>
       <c r="O37" s="6">
         <f t="shared" si="19"/>
-        <v>20.74074074074074</v>
+        <v>19.012345679012345</v>
       </c>
       <c r="P37" s="6">
         <f t="shared" si="20"/>
@@ -6219,7 +6132,7 @@
       <c r="R37" s="6"/>
       <c r="S37" s="6">
         <f t="shared" si="11"/>
-        <v>2.3821571238348866</v>
+        <v>1.4991122947181534</v>
       </c>
       <c r="T37" s="6">
         <f t="shared" si="12"/>
@@ -6227,11 +6140,11 @@
       </c>
       <c r="U37" s="6">
         <f t="shared" si="13"/>
-        <v>3.0343434343434348</v>
+        <v>2.7814814814814817</v>
       </c>
       <c r="V37" s="6">
         <f t="shared" si="22"/>
-        <v>1.9038461538461537</v>
+        <v>2.0769230769230771</v>
       </c>
       <c r="W37" s="6"/>
       <c r="X37" s="6"/>
@@ -6245,30 +6158,30 @@
         <v>float</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C39" s="8">
         <f>1/(C27*0.000001)</f>
         <v>1607.7170418006433</v>
       </c>
       <c r="D39" s="8">
-        <f t="shared" ref="D39:G39" si="32">1/(D27*0.000001)</f>
-        <v>4454.5414049623596</v>
+        <f t="shared" ref="D39:G39" si="33">1/(D27*0.000001)</f>
+        <v>4415.5958846646354</v>
       </c>
       <c r="E39" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>12939.958592132507</v>
       </c>
       <c r="F39" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>13958.682300390843</v>
       </c>
       <c r="G39" s="8">
-        <f t="shared" si="32"/>
-        <v>16126.431220770844</v>
+        <f t="shared" si="33"/>
+        <v>17226.528854435834</v>
       </c>
       <c r="H39" s="8">
-        <f t="shared" ref="H39" si="33">1/(H27*0.000001)</f>
+        <f t="shared" ref="H39" si="34">1/(H27*0.000001)</f>
         <v>384615.38461538462</v>
       </c>
       <c r="I39" s="8">
@@ -6279,27 +6192,27 @@
         <v>4</v>
       </c>
       <c r="K39" s="9">
-        <f t="shared" ref="K39:P39" si="34">$C$36/C28</f>
+        <f t="shared" ref="K39:P39" si="35">$C$36/C28</f>
         <v>0.12204724409448819</v>
       </c>
       <c r="L39" s="9">
-        <f t="shared" si="34"/>
-        <v>0.34267017443017267</v>
+        <f t="shared" si="35"/>
+        <v>0.3471833351999104</v>
       </c>
       <c r="M39" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0005163955589982</v>
       </c>
       <c r="N39" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0806665272258245</v>
       </c>
       <c r="O39" s="9">
-        <f t="shared" si="34"/>
-        <v>1.2410921611017696</v>
+        <f t="shared" si="35"/>
+        <v>1.3417590027700832</v>
       </c>
       <c r="P39" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>30.3921568627451</v>
       </c>
       <c r="Q39" s="9">
@@ -6313,61 +6226,61 @@
         <v>int32</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C40" s="8">
         <f>1/(C31*0.000001)</f>
         <v>3937.0078740157483</v>
       </c>
       <c r="D40" s="8">
-        <f t="shared" ref="D40:G40" si="35">1/(D31*0.000001)</f>
-        <v>38550.501156515034</v>
+        <f t="shared" ref="D40:G40" si="36">1/(D31*0.000001)</f>
+        <v>48100.048100048101</v>
       </c>
       <c r="E40" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>86132.644272179168</v>
       </c>
       <c r="F40" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>79365.079365079364</v>
       </c>
       <c r="G40" s="8">
-        <f t="shared" si="35"/>
-        <v>261780.10471204188</v>
+        <f t="shared" si="36"/>
+        <v>240384.61538461538</v>
       </c>
       <c r="H40" s="8">
-        <f t="shared" ref="H40" si="36">1/(H31*0.000001)</f>
+        <f t="shared" ref="H40" si="37">1/(H31*0.000001)</f>
         <v>500000</v>
       </c>
       <c r="I40" s="8">
-        <f t="shared" ref="I40" si="37">1/(I31*0.000001)</f>
+        <f t="shared" ref="I40" si="38">1/(I31*0.000001)</f>
         <v>175662.02626147293</v>
       </c>
       <c r="J40" t="s">
         <v>4</v>
       </c>
       <c r="K40" s="9">
-        <f t="shared" ref="K40:P40" si="38">$C$36/C32</f>
+        <f t="shared" ref="K40:P40" si="39">$C$36/C32</f>
         <v>0.30815109343936381</v>
       </c>
       <c r="L40" s="9">
-        <f t="shared" si="38"/>
-        <v>2.8719659069853622</v>
+        <f t="shared" si="39"/>
+        <v>3.7962282635317171</v>
       </c>
       <c r="M40" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.8101933216168709</v>
       </c>
       <c r="N40" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.25</v>
       </c>
       <c r="O40" s="9">
-        <f t="shared" si="38"/>
-        <v>20.666666666666668</v>
+        <f t="shared" si="39"/>
+        <v>18.971848225214199</v>
       </c>
       <c r="P40" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>39.743589743589745</v>
       </c>
       <c r="Q40" s="9">
@@ -6381,34 +6294,34 @@
         <v>int16</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C41" s="8">
         <f>1/(C35*0.000001)</f>
         <v>12658.227848101267</v>
       </c>
       <c r="D41" s="8">
-        <f t="shared" ref="D41:G41" si="39">1/(D35*0.000001)</f>
-        <v>38550.501156515034</v>
+        <f t="shared" ref="D41:G41" si="40">1/(D35*0.000001)</f>
+        <v>57273.768613974804</v>
       </c>
       <c r="E41" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>86132.644272179168</v>
       </c>
       <c r="F41" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>79365.079365079364</v>
       </c>
       <c r="G41" s="8">
-        <f t="shared" si="39"/>
-        <v>261780.10471204188</v>
+        <f t="shared" si="40"/>
+        <v>240384.61538461538</v>
       </c>
       <c r="H41" s="8">
-        <f t="shared" ref="H41" si="40">1/(H35*0.000001)</f>
+        <f t="shared" ref="H41" si="41">1/(H35*0.000001)</f>
         <v>500000</v>
       </c>
       <c r="I41" s="8">
-        <f t="shared" ref="I41" si="41">1/(I35*0.000001)</f>
+        <f t="shared" ref="I41" si="42">1/(I35*0.000001)</f>
         <v>175662.02626147293</v>
       </c>
       <c r="J41" t="s">
@@ -6419,23 +6332,23 @@
         <v>1</v>
       </c>
       <c r="L41" s="9">
-        <f t="shared" ref="L41:P41" si="42">$C$36/D36</f>
-        <v>2.8724981467753889</v>
+        <f t="shared" ref="L41:P41" si="43">$C$36/D36</f>
+        <v>4.5387994143484631</v>
       </c>
       <c r="M41" s="9">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>6.8101933216168709</v>
       </c>
       <c r="N41" s="9">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>6.25</v>
       </c>
       <c r="O41" s="9">
-        <f t="shared" si="42"/>
-        <v>20.666666666666668</v>
+        <f t="shared" si="43"/>
+        <v>18.971848225214199</v>
       </c>
       <c r="P41" s="9">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>39.743589743589745</v>
       </c>
       <c r="Q41" s="9">
@@ -6445,7 +6358,7 @@
     </row>
     <row r="59" spans="2:10">
       <c r="B59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G59">
         <v>250</v>
@@ -6460,23 +6373,23 @@
         <v>Arduino Uno</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" ref="D60:H60" si="43">D23</f>
+        <f t="shared" ref="D60:H60" si="44">D23</f>
         <v>Arduino M0 Pro</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Maple</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Arduino Due</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Teensy 3.1</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>K66F</v>
       </c>
       <c r="I60" t="str">
@@ -6494,23 +6407,23 @@
         <v>3549.4260376644552</v>
       </c>
       <c r="D61" s="8">
-        <f t="shared" ref="D61:G61" si="44">SQRT($G$59/((D28*0.000001)/$B28))</f>
-        <v>5947.4704793272776</v>
+        <f t="shared" ref="D61:G61" si="45">SQRT($G$59/((D28*0.000001)/$B28))</f>
+        <v>5986.5081443669142</v>
       </c>
       <c r="E61" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>10162.633113501566</v>
       </c>
       <c r="F61" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>10561.849922156138</v>
       </c>
       <c r="G61" s="8">
-        <f t="shared" si="44"/>
-        <v>11318.689818636485</v>
+        <f t="shared" si="45"/>
+        <v>11768.778828946262</v>
       </c>
       <c r="H61" s="8">
-        <f t="shared" ref="H61" si="45">SQRT($G$59/((H28*0.000001)/$B28))</f>
+        <f t="shared" ref="H61" si="46">SQRT($G$59/((H28*0.000001)/$B28))</f>
         <v>56011.203361120395</v>
       </c>
       <c r="I61" s="8">
@@ -6518,7 +6431,7 @@
         <v>76361.22447565374</v>
       </c>
       <c r="J61" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="2:10">
@@ -6531,23 +6444,23 @@
         <v>5639.9596744324917</v>
       </c>
       <c r="D62" s="8">
-        <f t="shared" ref="D62:G62" si="46">SQRT($G$59/((D32*0.000001)/$B32))</f>
-        <v>17218.042770596836</v>
+        <f t="shared" ref="D62:G62" si="47">SQRT($G$59/((D32*0.000001)/$B32))</f>
+        <v>19795.674375415139</v>
       </c>
       <c r="E62" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>26513.915171382934</v>
       </c>
       <c r="F62" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>25400.025400038103</v>
       </c>
       <c r="G62" s="8">
-        <f t="shared" si="46"/>
-        <v>46188.021535170061</v>
+        <f t="shared" si="47"/>
+        <v>44253.636380814365</v>
       </c>
       <c r="H62" s="8">
-        <f t="shared" ref="H62" si="47">SQRT($G$59/((H32*0.000001)/$B32))</f>
+        <f t="shared" ref="H62" si="48">SQRT($G$59/((H32*0.000001)/$B32))</f>
         <v>64051.261522034853</v>
       </c>
       <c r="I62" s="8">
@@ -6555,7 +6468,7 @@
         <v>76361.22447565374</v>
       </c>
       <c r="J62" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="2:10">
@@ -6568,23 +6481,23 @@
         <v>10160.010160015239</v>
       </c>
       <c r="D63" s="8">
-        <f t="shared" ref="D63:G63" si="48">SQRT($G$59/((D36*0.000001)/$B36))</f>
-        <v>17219.638141716368</v>
+        <f t="shared" ref="D63:G63" si="49">SQRT($G$59/((D36*0.000001)/$B36))</f>
+        <v>21645.351229957632</v>
       </c>
       <c r="E63" s="8">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>26513.915171382934</v>
       </c>
       <c r="F63" s="8">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>25400.025400038103</v>
       </c>
       <c r="G63" s="8">
-        <f t="shared" si="48"/>
-        <v>46188.021535170061</v>
+        <f t="shared" si="49"/>
+        <v>44253.636380814365</v>
       </c>
       <c r="H63" s="8">
-        <f t="shared" ref="H63" si="49">SQRT($G$59/((H36*0.000001)/$B36))</f>
+        <f t="shared" ref="H63" si="50">SQRT($G$59/((H36*0.000001)/$B36))</f>
         <v>64051.261522034853</v>
       </c>
       <c r="I63" s="8">
@@ -6592,58 +6505,58 @@
         <v>76361.22447565374</v>
       </c>
       <c r="J63" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C26:I37">
-    <cfRule type="cellIs" dxfId="29" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>$D$21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="12" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="12" stopIfTrue="1" operator="lessThan">
       <formula>$D$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="13" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="lessThan">
       <formula>$D$19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="14" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="14" stopIfTrue="1" operator="lessThan">
       <formula>$D$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="15" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="15" stopIfTrue="1" operator="greaterThan">
       <formula>$D$18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39:I41">
-    <cfRule type="cellIs" dxfId="24" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>$C$21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="7" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>$C$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="8" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="greaterThan">
       <formula>$C$19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="9" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" stopIfTrue="1" operator="greaterThan">
       <formula>$C$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>$C$18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:I63">
-    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>$C$21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>$C$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>$C$19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>$C$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>$C$18</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7157,7 +7070,7 @@
   <dimension ref="B2:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7207,10 +7120,10 @@
         <v>17</v>
       </c>
       <c r="L8" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="M8" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -7279,6 +7192,15 @@
         <f>H11/E11</f>
         <v>1.0286600949251552</v>
       </c>
+      <c r="K11">
+        <v>59.51</v>
+      </c>
+      <c r="L11">
+        <v>4.93</v>
+      </c>
+      <c r="M11">
+        <v>5.77</v>
+      </c>
     </row>
     <row r="12" spans="2:15">
       <c r="B12">
@@ -7302,17 +7224,17 @@
         <v>1.0151168117269811</v>
       </c>
       <c r="K12">
-        <v>112.4</v>
+        <v>114.83</v>
       </c>
       <c r="L12">
-        <v>13.26</v>
+        <v>9.11</v>
       </c>
       <c r="M12">
-        <v>13.26</v>
+        <v>10.77</v>
       </c>
       <c r="O12">
         <f>K12/L12</f>
-        <v>8.4766214177978885</v>
+        <v>12.604829857299672</v>
       </c>
     </row>
     <row r="13" spans="2:15">
@@ -7337,17 +7259,17 @@
         <v>1.0111688192305925</v>
       </c>
       <c r="K13">
-        <v>224.49</v>
+        <v>226.47</v>
       </c>
       <c r="L13">
-        <v>25.94</v>
+        <v>17.46</v>
       </c>
       <c r="M13">
-        <v>25.94</v>
+        <v>20.79</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13:O15" si="3">K13/L13</f>
-        <v>8.6542020046260593</v>
+        <f t="shared" ref="O13:O16" si="3">K13/L13</f>
+        <v>12.970790378006873</v>
       </c>
     </row>
     <row r="14" spans="2:15">
@@ -7372,17 +7294,17 @@
         <v>0.99981738495252015</v>
       </c>
       <c r="K14">
-        <v>452.33</v>
+        <v>446.45</v>
       </c>
       <c r="L14">
-        <v>53.96</v>
+        <v>34.15</v>
       </c>
       <c r="M14">
-        <v>53.97</v>
+        <v>40.83</v>
       </c>
       <c r="O14">
         <f t="shared" si="3"/>
-        <v>8.3826908821349146</v>
+        <v>13.07320644216691</v>
       </c>
     </row>
     <row r="15" spans="2:15">
@@ -7407,17 +7329,17 @@
         <v>0.99958845854863043</v>
       </c>
       <c r="K15">
-        <v>903.68</v>
+        <v>892.74</v>
       </c>
       <c r="L15">
-        <v>107.34</v>
+        <v>67.55</v>
       </c>
       <c r="M15">
-        <v>107.35</v>
+        <v>80.91</v>
       </c>
       <c r="O15">
         <f t="shared" si="3"/>
-        <v>8.4188559716787772</v>
+        <v>13.215988156920799</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -7441,8 +7363,21 @@
         <f t="shared" si="2"/>
         <v>0.99705215419501136</v>
       </c>
-    </row>
-    <row r="17" spans="2:9">
+      <c r="K16">
+        <v>1783.68</v>
+      </c>
+      <c r="L16">
+        <v>134.35</v>
+      </c>
+      <c r="M16">
+        <v>161.06</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>13.276367696315594</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
       <c r="B17">
         <v>512</v>
       </c>
@@ -7457,8 +7392,17 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="K17">
+        <v>3567.42</v>
+      </c>
+      <c r="L17">
+        <v>267.93</v>
+      </c>
+      <c r="M17">
+        <v>321.36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
       <c r="B18">
         <v>1024</v>
       </c>
@@ -7473,8 +7417,17 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="20" spans="2:9">
+      <c r="K18">
+        <v>7131.84</v>
+      </c>
+      <c r="L18">
+        <v>535.12</v>
+      </c>
+      <c r="M18">
+        <v>641.98</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
@@ -7485,7 +7438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:13">
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
@@ -7887,22 +7840,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K40"/>
+  <dimension ref="B2:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -7910,178 +7863,130 @@
         <v>46</v>
       </c>
     </row>
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="6" spans="2:6">
-      <c r="C6" t="s">
-        <v>51</v>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>14.87</v>
+      </c>
+      <c r="D6">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="C7" t="s">
-        <v>47</v>
+      <c r="B7" s="5">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>29.24</v>
+      </c>
+      <c r="D7">
+        <v>2.16</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
+      <c r="B8" s="5">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>58.05</v>
+      </c>
+      <c r="D8">
+        <v>4.16</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9">
-        <v>4</v>
+      <c r="B9" s="5">
+        <v>64</v>
       </c>
       <c r="C9">
-        <v>11.78</v>
+        <v>115.52</v>
       </c>
       <c r="D9">
-        <v>6.81</v>
-      </c>
-      <c r="E9">
-        <v>0.61</v>
-      </c>
-      <c r="F9">
-        <v>0.61</v>
+        <v>8.17</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10">
-        <v>8</v>
+      <c r="B10" s="5">
+        <v>128</v>
       </c>
       <c r="C10">
-        <v>24.81</v>
+        <v>230.49</v>
       </c>
       <c r="D10">
-        <v>14.74</v>
-      </c>
-      <c r="E10">
-        <v>1.07</v>
-      </c>
-      <c r="F10">
-        <v>1.07</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11">
-        <v>16</v>
+      <c r="B11" s="5">
+        <v>256</v>
       </c>
       <c r="C11">
-        <v>50.7</v>
+        <v>460.29</v>
       </c>
       <c r="D11">
-        <v>30.53</v>
-      </c>
-      <c r="E11">
-        <v>1.99</v>
-      </c>
-      <c r="F11">
-        <v>1.99</v>
+        <v>32.229999999999997</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12">
-        <v>32</v>
+      <c r="B12" s="5">
+        <v>512</v>
       </c>
       <c r="C12">
-        <v>102.3</v>
+        <v>919.99</v>
       </c>
       <c r="D12">
-        <v>62.01</v>
-      </c>
-      <c r="E12">
-        <v>3.82</v>
-      </c>
-      <c r="F12">
-        <v>3.82</v>
+        <v>64.31</v>
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13">
-        <v>64</v>
+      <c r="B13" s="5">
+        <v>1024</v>
       </c>
       <c r="C13">
-        <v>205.35</v>
+        <v>1839.32</v>
       </c>
       <c r="D13">
-        <v>124.89</v>
-      </c>
-      <c r="E13">
-        <v>7.5</v>
-      </c>
-      <c r="F13">
-        <v>7.5</v>
+        <v>128.49</v>
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14">
-        <v>128</v>
-      </c>
-      <c r="C14">
-        <v>411.28</v>
-      </c>
-      <c r="D14">
-        <v>250.57</v>
-      </c>
-      <c r="E14">
-        <v>14.85</v>
-      </c>
-      <c r="F14">
-        <v>14.85</v>
-      </c>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15">
-        <v>256</v>
-      </c>
-      <c r="C15">
-        <v>822.97</v>
-      </c>
-      <c r="D15">
-        <v>501.85</v>
-      </c>
-      <c r="E15">
-        <v>29.55</v>
-      </c>
-      <c r="F15">
-        <v>29.55</v>
-      </c>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16">
-        <v>512</v>
-      </c>
-      <c r="C16">
-        <v>1646.22</v>
-      </c>
-      <c r="D16">
-        <v>1004.33</v>
-      </c>
-      <c r="E16">
-        <v>58.96</v>
-      </c>
-      <c r="F16">
-        <v>58.96</v>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="C18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:8">
       <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19">
-        <f>96/72</f>
-        <v>1.3333333333333333</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:8">
@@ -8103,20 +8008,16 @@
         <v>4</v>
       </c>
       <c r="C21">
-        <v>12.67</v>
+        <v>11.78</v>
       </c>
       <c r="D21">
-        <v>7.36</v>
+        <v>6.81</v>
       </c>
       <c r="E21">
-        <v>0.81</v>
+        <v>0.61</v>
       </c>
       <c r="F21">
-        <v>0.81</v>
-      </c>
-      <c r="H21">
-        <f>F21/F9</f>
-        <v>1.3278688524590165</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -8124,20 +8025,16 @@
         <v>8</v>
       </c>
       <c r="C22">
-        <v>26.53</v>
+        <v>24.81</v>
       </c>
       <c r="D22">
-        <v>15.51</v>
+        <v>14.74</v>
       </c>
       <c r="E22">
-        <v>1.42</v>
+        <v>1.07</v>
       </c>
       <c r="F22">
-        <v>1.42</v>
-      </c>
-      <c r="H22">
-        <f t="shared" ref="H22:H28" si="0">F22/F10</f>
-        <v>1.3271028037383177</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -8145,20 +8042,16 @@
         <v>16</v>
       </c>
       <c r="C23">
-        <v>54.1</v>
+        <v>50.7</v>
       </c>
       <c r="D23">
-        <v>31.67</v>
+        <v>30.53</v>
       </c>
       <c r="E23">
-        <v>2.65</v>
+        <v>1.99</v>
       </c>
       <c r="F23">
-        <v>2.65</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
-        <v>1.3316582914572863</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -8166,20 +8059,16 @@
         <v>32</v>
       </c>
       <c r="C24">
-        <v>109.06</v>
+        <v>102.3</v>
       </c>
       <c r="D24">
-        <v>63.87</v>
+        <v>62.01</v>
       </c>
       <c r="E24">
-        <v>5.0999999999999996</v>
+        <v>3.82</v>
       </c>
       <c r="F24">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>1.3350785340314135</v>
+        <v>3.82</v>
       </c>
     </row>
     <row r="25" spans="2:8">
@@ -8187,20 +8076,16 @@
         <v>64</v>
       </c>
       <c r="C25">
-        <v>218.82</v>
+        <v>205.35</v>
       </c>
       <c r="D25">
-        <v>128.22</v>
+        <v>124.89</v>
       </c>
       <c r="E25">
-        <v>10</v>
+        <v>7.5</v>
       </c>
       <c r="F25">
-        <v>10</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="26" spans="2:8">
@@ -8208,20 +8093,16 @@
         <v>128</v>
       </c>
       <c r="C26">
-        <v>438.17</v>
+        <v>411.28</v>
       </c>
       <c r="D26">
-        <v>256.58</v>
+        <v>250.57</v>
       </c>
       <c r="E26">
-        <v>19.809999999999999</v>
+        <v>14.85</v>
       </c>
       <c r="F26">
-        <v>19.809999999999999</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>1.3340067340067339</v>
+        <v>14.85</v>
       </c>
     </row>
     <row r="27" spans="2:8">
@@ -8229,20 +8110,16 @@
         <v>256</v>
       </c>
       <c r="C27">
-        <v>876.73</v>
+        <v>822.97</v>
       </c>
       <c r="D27">
-        <v>513.32000000000005</v>
+        <v>501.85</v>
       </c>
       <c r="E27">
-        <v>39.43</v>
+        <v>29.55</v>
       </c>
       <c r="F27">
-        <v>39.43</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>1.3343485617597293</v>
+        <v>29.55</v>
       </c>
     </row>
     <row r="28" spans="2:8">
@@ -8250,30 +8127,30 @@
         <v>512</v>
       </c>
       <c r="C28">
-        <v>1753.6</v>
+        <v>1646.22</v>
       </c>
       <c r="D28">
-        <v>1026.67</v>
+        <v>1004.33</v>
       </c>
       <c r="E28">
-        <v>78.650000000000006</v>
+        <v>58.96</v>
       </c>
       <c r="F28">
-        <v>78.650000000000006</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
-        <v>1.3339552238805972</v>
+        <v>58.96</v>
       </c>
     </row>
     <row r="30" spans="2:8">
       <c r="C30" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="2:8">
       <c r="C31" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="H31">
+        <f>96/72</f>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="32" spans="2:8">
@@ -8289,40 +8166,37 @@
       <c r="F32" t="s">
         <v>22</v>
       </c>
-      <c r="H32" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="33" spans="2:11">
       <c r="B33">
         <v>4</v>
       </c>
       <c r="C33">
-        <v>12.36</v>
+        <v>12.67</v>
       </c>
       <c r="D33">
-        <v>7.95</v>
+        <v>7.36</v>
       </c>
       <c r="E33">
-        <v>0.89</v>
+        <v>0.81</v>
       </c>
       <c r="F33">
-        <v>0.89</v>
+        <v>0.81</v>
       </c>
       <c r="H33">
-        <f>C33/C9</f>
-        <v>1.0492359932088284</v>
+        <f>F33/F21</f>
+        <v>1.3278688524590165</v>
       </c>
       <c r="I33">
-        <f t="shared" ref="I33:K40" si="1">D33/D9</f>
+        <f t="shared" ref="I33:K40" si="0">D45/D21</f>
         <v>1.1674008810572689</v>
       </c>
       <c r="J33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.459016393442623</v>
       </c>
       <c r="K33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.459016393442623</v>
       </c>
     </row>
@@ -8331,31 +8205,31 @@
         <v>8</v>
       </c>
       <c r="C34">
-        <v>25.72</v>
+        <v>26.53</v>
       </c>
       <c r="D34">
-        <v>16.88</v>
+        <v>15.51</v>
       </c>
       <c r="E34">
-        <v>1.56</v>
+        <v>1.42</v>
       </c>
       <c r="F34">
-        <v>1.56</v>
+        <v>1.42</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H40" si="2">C34/C10</f>
-        <v>1.0366787585650947</v>
+        <f t="shared" ref="H34:H40" si="1">F34/F22</f>
+        <v>1.3271028037383177</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1451831750339212</v>
       </c>
       <c r="J34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4579439252336448</v>
       </c>
       <c r="K34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4579439252336448</v>
       </c>
     </row>
@@ -8364,31 +8238,31 @@
         <v>16</v>
       </c>
       <c r="C35">
-        <v>52.28</v>
+        <v>54.1</v>
       </c>
       <c r="D35">
-        <v>34.659999999999997</v>
+        <v>31.67</v>
       </c>
       <c r="E35">
-        <v>2.89</v>
+        <v>2.65</v>
       </c>
       <c r="F35">
-        <v>2.89</v>
+        <v>2.65</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
-        <v>1.031163708086785</v>
+        <f t="shared" si="1"/>
+        <v>1.3316582914572863</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1352767769407139</v>
       </c>
       <c r="J35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4522613065326633</v>
       </c>
       <c r="K35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4522613065326633</v>
       </c>
     </row>
@@ -8397,31 +8271,31 @@
         <v>32</v>
       </c>
       <c r="C36">
-        <v>105.2</v>
+        <v>109.06</v>
       </c>
       <c r="D36">
-        <v>70.22</v>
+        <v>63.87</v>
       </c>
       <c r="E36">
-        <v>5.56</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F36">
-        <v>5.56</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H36">
-        <f t="shared" si="2"/>
-        <v>1.0283479960899315</v>
+        <f t="shared" si="1"/>
+        <v>1.3350785340314135</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1323980003225287</v>
       </c>
       <c r="J36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4554973821989527</v>
       </c>
       <c r="K36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4554973821989527</v>
       </c>
     </row>
@@ -8430,31 +8304,31 @@
         <v>64</v>
       </c>
       <c r="C37">
-        <v>210.9</v>
+        <v>218.82</v>
       </c>
       <c r="D37">
-        <v>141.04</v>
+        <v>128.22</v>
       </c>
       <c r="E37">
-        <v>10.91</v>
+        <v>10</v>
       </c>
       <c r="F37">
-        <v>10.91</v>
+        <v>10</v>
       </c>
       <c r="H37">
-        <f t="shared" si="2"/>
-        <v>1.027027027027027</v>
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1293137961406037</v>
       </c>
       <c r="J37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4546666666666668</v>
       </c>
       <c r="K37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4546666666666668</v>
       </c>
     </row>
@@ -8463,31 +8337,31 @@
         <v>128</v>
       </c>
       <c r="C38">
-        <v>422.11</v>
+        <v>438.17</v>
       </c>
       <c r="D38">
-        <v>282.75</v>
+        <v>256.58</v>
       </c>
       <c r="E38">
-        <v>21.6</v>
+        <v>19.809999999999999</v>
       </c>
       <c r="F38">
-        <v>21.6</v>
+        <v>19.809999999999999</v>
       </c>
       <c r="H38">
-        <f t="shared" si="2"/>
-        <v>1.0263324255981328</v>
+        <f t="shared" si="1"/>
+        <v>1.3340067340067339</v>
       </c>
       <c r="I38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1284271860158839</v>
       </c>
       <c r="J38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4545454545454546</v>
       </c>
       <c r="K38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4545454545454546</v>
       </c>
     </row>
@@ -8496,31 +8370,31 @@
         <v>256</v>
       </c>
       <c r="C39">
-        <v>844.39</v>
+        <v>876.73</v>
       </c>
       <c r="D39">
-        <v>566.07000000000005</v>
+        <v>513.32000000000005</v>
       </c>
       <c r="E39">
-        <v>42.97</v>
+        <v>39.43</v>
       </c>
       <c r="F39">
-        <v>42.97</v>
+        <v>39.43</v>
       </c>
       <c r="H39">
-        <f t="shared" si="2"/>
-        <v>1.026027680231357</v>
+        <f t="shared" si="1"/>
+        <v>1.3343485617597293</v>
       </c>
       <c r="I39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1279665238617118</v>
       </c>
       <c r="J39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4541455160744501</v>
       </c>
       <c r="K39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4541455160744501</v>
       </c>
     </row>
@@ -8529,32 +8403,227 @@
         <v>512</v>
       </c>
       <c r="C40">
+        <v>1753.6</v>
+      </c>
+      <c r="D40">
+        <v>1026.67</v>
+      </c>
+      <c r="E40">
+        <v>78.650000000000006</v>
+      </c>
+      <c r="F40">
+        <v>78.650000000000006</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>1.3339552238805972</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>1.127766769886392</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>1.4536974219810039</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>1.4536974219810039</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11">
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11">
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>12.36</v>
+      </c>
+      <c r="D45">
+        <v>7.95</v>
+      </c>
+      <c r="E45">
+        <v>0.89</v>
+      </c>
+      <c r="F45">
+        <v>0.89</v>
+      </c>
+      <c r="H45">
+        <f>C45/C21</f>
+        <v>1.0492359932088284</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>25.72</v>
+      </c>
+      <c r="D46">
+        <v>16.88</v>
+      </c>
+      <c r="E46">
+        <v>1.56</v>
+      </c>
+      <c r="F46">
+        <v>1.56</v>
+      </c>
+      <c r="H46">
+        <f t="shared" ref="H46:H52" si="2">C46/C22</f>
+        <v>1.0366787585650947</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47">
+        <v>16</v>
+      </c>
+      <c r="C47">
+        <v>52.28</v>
+      </c>
+      <c r="D47">
+        <v>34.659999999999997</v>
+      </c>
+      <c r="E47">
+        <v>2.89</v>
+      </c>
+      <c r="F47">
+        <v>2.89</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="2"/>
+        <v>1.031163708086785</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="B48">
+        <v>32</v>
+      </c>
+      <c r="C48">
+        <v>105.2</v>
+      </c>
+      <c r="D48">
+        <v>70.22</v>
+      </c>
+      <c r="E48">
+        <v>5.56</v>
+      </c>
+      <c r="F48">
+        <v>5.56</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="2"/>
+        <v>1.0283479960899315</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49">
+        <v>64</v>
+      </c>
+      <c r="C49">
+        <v>210.9</v>
+      </c>
+      <c r="D49">
+        <v>141.04</v>
+      </c>
+      <c r="E49">
+        <v>10.91</v>
+      </c>
+      <c r="F49">
+        <v>10.91</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="2"/>
+        <v>1.027027027027027</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50">
+        <v>128</v>
+      </c>
+      <c r="C50">
+        <v>422.11</v>
+      </c>
+      <c r="D50">
+        <v>282.75</v>
+      </c>
+      <c r="E50">
+        <v>21.6</v>
+      </c>
+      <c r="F50">
+        <v>21.6</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="2"/>
+        <v>1.0263324255981328</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51">
+        <v>256</v>
+      </c>
+      <c r="C51">
+        <v>844.39</v>
+      </c>
+      <c r="D51">
+        <v>566.07000000000005</v>
+      </c>
+      <c r="E51">
+        <v>42.97</v>
+      </c>
+      <c r="F51">
+        <v>42.97</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="2"/>
+        <v>1.026027680231357</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52">
+        <v>512</v>
+      </c>
+      <c r="C52">
         <v>1688.76</v>
       </c>
-      <c r="D40">
+      <c r="D52">
         <v>1132.6500000000001</v>
       </c>
-      <c r="E40">
+      <c r="E52">
         <v>85.71</v>
       </c>
-      <c r="F40">
+      <c r="F52">
         <v>85.71</v>
       </c>
-      <c r="H40">
+      <c r="H52">
         <f t="shared" si="2"/>
         <v>1.0258410176039654</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="1"/>
-        <v>1.127766769886392</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="1"/>
-        <v>1.4536974219810039</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="1"/>
-        <v>1.4536974219810039</v>
       </c>
     </row>
   </sheetData>
@@ -8580,22 +8649,22 @@
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="C5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="C6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="2:6">
@@ -8741,7 +8810,7 @@
   <sheetData>
     <row r="6" spans="2:11">
       <c r="C6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" t="str">
         <f>C6</f>
@@ -8750,7 +8819,7 @@
     </row>
     <row r="7" spans="2:11">
       <c r="C7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" t="str">
         <f>C7</f>
@@ -8759,16 +8828,16 @@
     </row>
     <row r="8" spans="2:11">
       <c r="C8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:11">

</xml_diff>